<commit_message>
Thêm cột ID vào bảng Quản trị viên, cập nhật tương tác cơ sở dữ liệu và tinh chỉnh mô hình dữ liệu cho phần ID để quản lý nhân viên
</commit_message>
<xml_diff>
--- a/BTLJavaFX/log.xlsx
+++ b/BTLJavaFX/log.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>Time</t>
   </si>
@@ -77,6 +77,81 @@
   </si>
   <si>
     <t>19-10-2025 22:20:20</t>
+  </si>
+  <si>
+    <t>20-10-2025 07:30:49</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Nam</t>
+  </si>
+  <si>
+    <t>20-10-2025 07:31:06</t>
+  </si>
+  <si>
+    <t>20-10-2025 07:31:11</t>
+  </si>
+  <si>
+    <t>20-10-2025 07:31:14</t>
+  </si>
+  <si>
+    <t>20-10-2025 07:38:38</t>
+  </si>
+  <si>
+    <t>20-10-2025 07:38:53</t>
+  </si>
+  <si>
+    <t>20-10-2025 07:38:55</t>
+  </si>
+  <si>
+    <t>20-10-2025 07:39:34</t>
+  </si>
+  <si>
+    <t>20-10-2025 07:39:49</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:17:49</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:18:13</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:38:14</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:39:39</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:53:32</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:53:45</t>
+  </si>
+  <si>
+    <t>Thêm nhân viên: Đặng Thị Thúy (Staff)</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:53:53</t>
+  </si>
+  <si>
+    <t>Quản lý xóa nhân viên: Đặng Thị Thúy</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:54:36</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:54:51</t>
+  </si>
+  <si>
+    <t>Thêm nhân viên: Phạm Thị Thúy (Staff)</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:54:55</t>
+  </si>
+  <si>
+    <t>20-10-2025 09:55:03</t>
+  </si>
+  <si>
+    <t>Phạm Thị Thúy</t>
   </si>
 </sst>
 </file>
@@ -449,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C6"/>
@@ -567,6 +642,226 @@
         <v>5</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create + delete food
</commit_message>
<xml_diff>
--- a/BTLJavaFX/log.xlsx
+++ b/BTLJavaFX/log.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="55">
   <si>
     <t>Time</t>
   </si>
@@ -152,6 +152,39 @@
   </si>
   <si>
     <t>Phạm Thị Thúy</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:16:01</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:19:55</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:27:53</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:28:08</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:29:01</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:30:26</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:31:24</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:32:43</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:33:46</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:34:33</t>
+  </si>
+  <si>
+    <t>20-10-2025 10:35:00</t>
   </si>
 </sst>
 </file>
@@ -524,7 +557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C6"/>
@@ -862,6 +895,127 @@
         <v>5</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>